<commit_message>
econ: anchor machines for wheeled harvester and forwarders
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios psme.xlsx
+++ b/UnitTests/financial scenarios psme.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="134">
   <si>
     <t>name</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>sitePrepPlant</t>
+  </si>
+  <si>
+    <t>anchorSMh</t>
+  </si>
+  <si>
+    <t>addOnWinchCableLength</t>
   </si>
 </sst>
 </file>
@@ -773,22 +779,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DG2"/>
+  <dimension ref="A1:DI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CZ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DE1" sqref="DE1:DG2"/>
+      <selection pane="bottomRight" activeCell="BF2" sqref="BF1:BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="15" max="24" width="8.88671875" customWidth="1"/>
-    <col min="106" max="111" width="8.88671875" customWidth="1"/>
+    <col min="108" max="113" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -961,169 +967,175 @@
         <v>73</v>
       </c>
       <c r="BF1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BG1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BX1" s="10" t="s">
+      <c r="BY1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="BY1" s="10" t="s">
+      <c r="BZ1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="CF1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1300,176 +1312,182 @@
       <c r="BE2" s="1">
         <v>0.79</v>
       </c>
-      <c r="BF2" s="1">
+      <c r="BF2" s="4">
+        <v>350</v>
+      </c>
+      <c r="BG2" s="1">
         <f>(180+30+25)/60</f>
         <v>3.9166666666666665</v>
       </c>
-      <c r="BG2" s="1">
-        <f>3/BF2*125</f>
+      <c r="BH2" s="1">
+        <f>3/BG2*125</f>
         <v>95.744680851063833</v>
       </c>
-      <c r="BH2" s="1">
+      <c r="BI2" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="BI2" s="1">
+      <c r="BJ2" s="1">
         <v>0.9</v>
       </c>
-      <c r="BJ2" s="1">
+      <c r="BK2" s="1">
         <v>1.5</v>
       </c>
-      <c r="BK2" s="1">
+      <c r="BL2" s="1">
         <v>0.35</v>
       </c>
-      <c r="BL2" s="4">
+      <c r="BM2" s="4">
         <v>14</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <v>4.7</v>
       </c>
-      <c r="BN2">
+      <c r="BO2">
         <v>30</v>
       </c>
-      <c r="BO2" s="5">
+      <c r="BP2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="BP2" s="1">
+      <c r="BQ2" s="1">
         <v>263</v>
       </c>
-      <c r="BQ2" s="1">
+      <c r="BR2" s="1">
         <v>0.77</v>
       </c>
-      <c r="BR2" s="4">
+      <c r="BS2" s="4">
         <v>105</v>
       </c>
-      <c r="BS2" s="4">
+      <c r="BT2" s="4">
         <v>80</v>
       </c>
-      <c r="BT2" s="4">
+      <c r="BU2" s="4">
         <v>28</v>
       </c>
-      <c r="BU2" s="4">
+      <c r="BV2" s="4">
         <v>43</v>
-      </c>
-      <c r="BV2" s="3">
-        <v>3</v>
       </c>
       <c r="BW2" s="3">
         <v>3</v>
       </c>
       <c r="BX2" s="3">
+        <v>3</v>
+      </c>
+      <c r="BY2" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BY2" s="3">
+      <c r="BZ2" s="3">
         <v>5</v>
       </c>
-      <c r="BZ2" s="4">
+      <c r="CA2" s="4">
         <v>30</v>
       </c>
-      <c r="CA2" s="1">
+      <c r="CB2" s="1">
         <v>0.01</v>
       </c>
-      <c r="CB2" s="1">
+      <c r="CC2" s="1">
         <v>264</v>
       </c>
-      <c r="CC2" s="1">
+      <c r="CD2" s="1">
         <v>0.77</v>
       </c>
-      <c r="CD2">
+      <c r="CE2" s="1">
+        <v>71.5</v>
+      </c>
+      <c r="CF2">
         <v>45</v>
       </c>
-      <c r="CE2">
+      <c r="CG2">
         <v>0.72</v>
       </c>
-      <c r="CF2">
+      <c r="CH2">
         <v>4000</v>
       </c>
-      <c r="CG2">
+      <c r="CI2">
         <v>2000</v>
       </c>
-      <c r="CH2" s="1">
+      <c r="CJ2" s="1">
         <v>360</v>
       </c>
-      <c r="CI2" s="1">
+      <c r="CK2" s="1">
         <v>0.8</v>
       </c>
-      <c r="CJ2">
+      <c r="CL2">
         <v>2900</v>
       </c>
-      <c r="CK2">
+      <c r="CM2">
         <v>1550</v>
       </c>
-      <c r="CL2" s="1">
+      <c r="CN2" s="1">
         <v>248</v>
       </c>
-      <c r="CM2">
+      <c r="CO2">
         <v>0.75</v>
       </c>
-      <c r="CN2">
+      <c r="CP2">
         <v>21</v>
       </c>
-      <c r="CO2">
+      <c r="CQ2">
         <v>30</v>
       </c>
-      <c r="CP2">
+      <c r="CR2">
         <v>1.5</v>
       </c>
-      <c r="CQ2">
+      <c r="CS2">
         <v>2.5</v>
       </c>
-      <c r="CR2">
+      <c r="CT2">
         <v>4.5</v>
       </c>
-      <c r="CS2" s="3">
+      <c r="CU2" s="3">
         <v>6</v>
       </c>
-      <c r="CT2" s="1">
+      <c r="CV2" s="1">
         <v>204</v>
       </c>
-      <c r="CU2" s="1">
+      <c r="CW2" s="1">
         <v>0.89</v>
       </c>
-      <c r="CV2" s="4">
-        <f>2*CY2</f>
+      <c r="CX2" s="4">
+        <f>2*DA2</f>
         <v>52024.5</v>
       </c>
-      <c r="CW2" s="1">
+      <c r="CY2" s="1">
         <v>172</v>
       </c>
-      <c r="CX2" s="1">
+      <c r="CZ2" s="1">
         <v>0.9</v>
       </c>
-      <c r="CY2" s="4">
+      <c r="DA2" s="4">
         <f>0.99*26275</f>
         <v>26012.25</v>
       </c>
-      <c r="CZ2" s="1">
+      <c r="DB2" s="1">
         <f>(180+17.5+17.5)/60</f>
         <v>3.5833333333333335</v>
       </c>
-      <c r="DA2" s="1">
-        <f>3/CZ2*100</f>
+      <c r="DC2" s="1">
+        <f>3/DB2*100</f>
         <v>83.720930232558132</v>
       </c>
-      <c r="DB2" s="1">
+      <c r="DD2" s="1">
         <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
         <v>520.33333333333326</v>
       </c>
-      <c r="DC2" s="1">
+      <c r="DE2" s="1">
         <v>1.5</v>
       </c>
-      <c r="DD2" s="1">
+      <c r="DF2" s="1">
         <f>0.35 + 0.12</f>
         <v>0.47</v>
       </c>
-      <c r="DE2" s="1">
+      <c r="DG2" s="1">
         <f>145+200+383</f>
         <v>728</v>
       </c>
-      <c r="DF2" s="1">
+      <c r="DH2" s="1">
         <v>0.5</v>
       </c>
-      <c r="DG2" s="1">
+      <c r="DI2" s="1">
         <v>275</v>
       </c>
     </row>

</xml_diff>